<commit_message>
Perhitungan manual astar dan jps di file animate
</commit_message>
<xml_diff>
--- a/Excel/Rekap/Rekap_Avg_SemuaSheet.xlsx
+++ b/Excel/Rekap/Rekap_Avg_SemuaSheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SEMHAS\TA_Python_Server\Excel\Rekap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E978C49-B03D-4CE7-BBDD-43F6881E9648}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FB528DF-C424-45F9-853F-B1890AB09627}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -57,196 +57,196 @@
     <t>Jumlah Belok</t>
   </si>
   <si>
+    <t>A*</t>
+  </si>
+  <si>
+    <t>BDS</t>
+  </si>
+  <si>
+    <t>BRC</t>
+  </si>
+  <si>
+    <t>GL</t>
+  </si>
+  <si>
+    <t>JPS</t>
+  </si>
+  <si>
+    <t>PPO</t>
+  </si>
+  <si>
+    <t>TPF</t>
+  </si>
+  <si>
+    <t>BDS-BRC</t>
+  </si>
+  <si>
+    <t>BDS-GL</t>
+  </si>
+  <si>
+    <t>BDS-PPO</t>
+  </si>
+  <si>
+    <t>BDS-TPF</t>
+  </si>
+  <si>
+    <t>BRC-PPO</t>
+  </si>
+  <si>
+    <t>BRC-TPF</t>
+  </si>
+  <si>
+    <t>GL-BRC</t>
+  </si>
+  <si>
+    <t>GL-PPO</t>
+  </si>
+  <si>
+    <t>GL-TPF</t>
+  </si>
+  <si>
+    <t>JPS-BDS</t>
+  </si>
+  <si>
+    <t>JPS-BRC</t>
+  </si>
+  <si>
+    <t>JPS-GL</t>
+  </si>
+  <si>
+    <t>JPS-PPO</t>
+  </si>
+  <si>
+    <t>JPS-TPF</t>
+  </si>
+  <si>
+    <t>TPF-PPO</t>
+  </si>
+  <si>
+    <t>BDS-BRC-PPO</t>
+  </si>
+  <si>
+    <t>BDS-BRC-TPF</t>
+  </si>
+  <si>
+    <t>BDS-GL-BRC</t>
+  </si>
+  <si>
+    <t>BDS-GL-PPO</t>
+  </si>
+  <si>
+    <t>BDS-GL-TPF</t>
+  </si>
+  <si>
+    <t>BDS-TPF-PPO</t>
+  </si>
+  <si>
+    <t>BRC-TPF-PPO</t>
+  </si>
+  <si>
+    <t>GL-BRC-PPO</t>
+  </si>
+  <si>
+    <t>GL-BRC-TPF</t>
+  </si>
+  <si>
+    <t>GL-TPF-PPO</t>
+  </si>
+  <si>
+    <t>JPS-BDS-BRC</t>
+  </si>
+  <si>
+    <t>JPS-BDS-GL</t>
+  </si>
+  <si>
+    <t>JPS-BDS-PPO</t>
+  </si>
+  <si>
+    <t>JPS-BDS-TPF</t>
+  </si>
+  <si>
+    <t>JPS-BRC-PPO</t>
+  </si>
+  <si>
     <t>JPS-BRC-TPF</t>
   </si>
   <si>
+    <t>JPS-GL-BRC</t>
+  </si>
+  <si>
+    <t>JPS-GL-PPO</t>
+  </si>
+  <si>
+    <t>JPS-GL-TPF</t>
+  </si>
+  <si>
+    <t>JPS-TPF-PPO</t>
+  </si>
+  <si>
+    <t>BDS-BRC-TPF-PPO</t>
+  </si>
+  <si>
+    <t>BDS-GL-BRC-PPO</t>
+  </si>
+  <si>
+    <t>BDS-GL-BRC-TPF</t>
+  </si>
+  <si>
+    <t>BDS-GL-TPF-PPO</t>
+  </si>
+  <si>
+    <t>GL-BRC-TPF-PPO</t>
+  </si>
+  <si>
+    <t>JPS-BDS-BRC-PPO</t>
+  </si>
+  <si>
+    <t>JPS-BDS-BRC-TPF</t>
+  </si>
+  <si>
+    <t>JPS-BDS-GL-BRC</t>
+  </si>
+  <si>
+    <t>JPS-BDS-GL-PPO</t>
+  </si>
+  <si>
+    <t>JPS-BDS-GL-TPF</t>
+  </si>
+  <si>
+    <t>JPS-BDS-TPF-PPO</t>
+  </si>
+  <si>
     <t>JPS-BRC-TPF-PPO</t>
   </si>
   <si>
-    <t>JPS-BRC</t>
-  </si>
-  <si>
-    <t>JPS-BRC-PPO</t>
-  </si>
-  <si>
-    <t>JPS-GL-BRC</t>
+    <t>JPS-GL-BRC-PPO</t>
   </si>
   <si>
     <t>JPS-GL-BRC-TPF</t>
   </si>
   <si>
-    <t>JPS-GL-BRC-PPO</t>
+    <t>JPS-GL-TPF-PPO</t>
+  </si>
+  <si>
+    <t>BDS-GL-BRC-TPF-PPO</t>
+  </si>
+  <si>
+    <t>JPS-BDS-BRC-TPF-PPO</t>
+  </si>
+  <si>
+    <t>JPS-BDS-GL-BRC-PPO</t>
+  </si>
+  <si>
+    <t>JPS-BDS-GL-BRC-TPF</t>
+  </si>
+  <si>
+    <t>JPS-BDS-GL-TPF-PPO</t>
   </si>
   <si>
     <t>JPS-GL-BRC-TPF-PPO</t>
   </si>
   <si>
-    <t>JPS-BDS-GL</t>
-  </si>
-  <si>
-    <t>JPS-BDS-GL-PPO</t>
-  </si>
-  <si>
-    <t>JPS-BDS-BRC</t>
-  </si>
-  <si>
-    <t>JPS-BDS-GL-BRC</t>
-  </si>
-  <si>
-    <t>JPS-BDS-BRC-PPO</t>
-  </si>
-  <si>
-    <t>JPS-BDS-GL-BRC-PPO</t>
-  </si>
-  <si>
-    <t>JPS-BDS-BRC-TPF</t>
-  </si>
-  <si>
-    <t>JPS-BDS-BRC-TPF-PPO</t>
-  </si>
-  <si>
-    <t>JPS-BDS</t>
-  </si>
-  <si>
-    <t>JPS-BDS-PPO</t>
-  </si>
-  <si>
-    <t>JPS-BDS-GL-BRC-TPF</t>
-  </si>
-  <si>
     <t>JPS-BDS-GL-BRC-TPF-PPO</t>
-  </si>
-  <si>
-    <t>JPS-BDS-GL-TPF</t>
-  </si>
-  <si>
-    <t>JPS-BDS-GL-TPF-PPO</t>
-  </si>
-  <si>
-    <t>JPS-BDS-TPF</t>
-  </si>
-  <si>
-    <t>JPS-BDS-TPF-PPO</t>
-  </si>
-  <si>
-    <t>JPS-GL</t>
-  </si>
-  <si>
-    <t>JPS-GL-PPO</t>
-  </si>
-  <si>
-    <t>JPS-GL-TPF</t>
-  </si>
-  <si>
-    <t>JPS-GL-TPF-PPO</t>
-  </si>
-  <si>
-    <t>BDS</t>
-  </si>
-  <si>
-    <t>BDS-PPO</t>
-  </si>
-  <si>
-    <t>BDS-TPF</t>
-  </si>
-  <si>
-    <t>BDS-TPF-PPO</t>
-  </si>
-  <si>
-    <t>JPS-TPF</t>
-  </si>
-  <si>
-    <t>JPS-TPF-PPO</t>
-  </si>
-  <si>
-    <t>JPS</t>
-  </si>
-  <si>
-    <t>JPS-PPO</t>
-  </si>
-  <si>
-    <t>BDS-GL</t>
-  </si>
-  <si>
-    <t>BDS-GL-TPF</t>
-  </si>
-  <si>
-    <t>BDS-GL-PPO</t>
-  </si>
-  <si>
-    <t>BDS-GL-TPF-PPO</t>
-  </si>
-  <si>
-    <t>BDS-BRC</t>
-  </si>
-  <si>
-    <t>BDS-BRC-PPO</t>
-  </si>
-  <si>
-    <t>BDS-BRC-TPF</t>
-  </si>
-  <si>
-    <t>BDS-BRC-TPF-PPO</t>
-  </si>
-  <si>
-    <t>BDS-GL-BRC-TPF</t>
-  </si>
-  <si>
-    <t>BDS-GL-BRC-TPF-PPO</t>
-  </si>
-  <si>
-    <t>BDS-GL-BRC</t>
-  </si>
-  <si>
-    <t>BDS-GL-BRC-PPO</t>
-  </si>
-  <si>
-    <t>BRC</t>
-  </si>
-  <si>
-    <t>BRC-PPO</t>
-  </si>
-  <si>
-    <t>BRC-TPF</t>
-  </si>
-  <si>
-    <t>BRC-TPF-PPO</t>
-  </si>
-  <si>
-    <t>GL-BRC-TPF</t>
-  </si>
-  <si>
-    <t>GL-BRC-TPF-PPO</t>
-  </si>
-  <si>
-    <t>GL-BRC</t>
-  </si>
-  <si>
-    <t>GL-BRC-PPO</t>
-  </si>
-  <si>
-    <t>GL-TPF</t>
-  </si>
-  <si>
-    <t>GL-TPF-PPO</t>
-  </si>
-  <si>
-    <t>GL</t>
-  </si>
-  <si>
-    <t>GL-PPO</t>
-  </si>
-  <si>
-    <t>TPF</t>
-  </si>
-  <si>
-    <t>TPF-PPO</t>
-  </si>
-  <si>
-    <t>A*</t>
-  </si>
-  <si>
-    <t>PPO</t>
   </si>
   <si>
     <t>avg</t>
@@ -634,7 +634,7 @@
   <dimension ref="A1:H65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -676,502 +676,502 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B2">
-        <v>4.22405E-3</v>
+        <v>5.8780910000000013E-2</v>
       </c>
       <c r="C2">
-        <v>11</v>
+        <v>80.25</v>
       </c>
       <c r="D2">
-        <v>97.253304076183326</v>
+        <v>95.466460966906681</v>
       </c>
       <c r="E2">
-        <v>11.75</v>
+        <v>265.10000000000002</v>
       </c>
       <c r="F2">
-        <v>26.95</v>
+        <v>1574.9</v>
       </c>
       <c r="G2">
-        <v>9</v>
+        <v>19.8</v>
       </c>
       <c r="H2">
-        <f>AVERAGE(B2,D2,E2,F2,G2)</f>
-        <v>28.991505625236663</v>
+        <f>AVERAGE(B2:G2)</f>
+        <v>339.2625403128178</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B3">
-        <v>4.4211249999999997E-3</v>
+        <v>6.821405E-3</v>
       </c>
       <c r="C3">
-        <v>11</v>
+        <v>80.25</v>
       </c>
       <c r="D3">
-        <v>97.253304076183326</v>
+        <v>96.046359954229004</v>
       </c>
       <c r="E3">
-        <v>11.65</v>
+        <v>304.85000000000002</v>
       </c>
       <c r="F3">
-        <v>27.55</v>
+        <v>1118.4000000000001</v>
       </c>
       <c r="G3">
-        <v>9</v>
+        <v>12.6</v>
       </c>
       <c r="H3">
-        <f>AVERAGE(B3,D3,E3,F3,G3)</f>
-        <v>29.091545040236667</v>
+        <f t="shared" ref="H3:H65" si="0">AVERAGE(B3:G3)</f>
+        <v>268.69219689320488</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B4">
-        <v>4.4850949999999997E-3</v>
+        <v>2.8290889999999999E-2</v>
       </c>
       <c r="C4">
-        <v>11.4</v>
+        <v>86.95</v>
       </c>
       <c r="D4">
-        <v>97.581102103629476</v>
+        <v>101.545140623347</v>
       </c>
       <c r="E4">
-        <v>12.45</v>
+        <v>228.45</v>
       </c>
       <c r="F4">
-        <v>27.75</v>
+        <v>456.95</v>
       </c>
       <c r="G4">
-        <v>9.4</v>
+        <v>16.7</v>
       </c>
       <c r="H4">
-        <f>AVERAGE(B4,D4,E4,F4,G4)</f>
-        <v>29.437117439725899</v>
+        <f t="shared" si="0"/>
+        <v>148.43723858555782</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B5">
-        <v>4.636935E-3</v>
+        <v>3.9248825000000001E-2</v>
       </c>
       <c r="C5">
-        <v>11.4</v>
+        <v>80.95</v>
       </c>
       <c r="D5">
-        <v>97.581102103629476</v>
+        <v>95.8765114732455</v>
       </c>
       <c r="E5">
-        <v>12.45</v>
+        <v>221.85</v>
       </c>
       <c r="F5">
-        <v>27.75</v>
+        <v>1060.95</v>
       </c>
       <c r="G5">
-        <v>9.4</v>
+        <v>11.7</v>
       </c>
       <c r="H5">
-        <f>AVERAGE(B5,D5,E5,F5,G5)</f>
-        <v>29.437147807725893</v>
+        <f t="shared" si="0"/>
+        <v>245.22762671637426</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B6">
-        <v>4.1160550000000004E-3</v>
+        <v>7.8221300000000001E-3</v>
       </c>
       <c r="C6">
-        <v>18.850000000000001</v>
+        <v>17.149999999999999</v>
       </c>
       <c r="D6">
-        <v>99.130927060973946</v>
+        <v>95.466460966906681</v>
       </c>
       <c r="E6">
-        <v>11.75</v>
+        <v>12.25</v>
       </c>
       <c r="F6">
-        <v>26.95</v>
+        <v>46.65</v>
       </c>
       <c r="G6">
-        <v>10.85</v>
+        <v>8.5</v>
       </c>
       <c r="H6">
-        <f>AVERAGE(B6,D6,E6,F6,G6)</f>
-        <v>29.737008623194789</v>
+        <f t="shared" si="0"/>
+        <v>30.004047182817782</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B7">
-        <v>4.264795E-3</v>
+        <v>5.8907709999999988E-2</v>
       </c>
       <c r="C7">
-        <v>18.850000000000001</v>
+        <v>8.75</v>
       </c>
       <c r="D7">
-        <v>99.130927060973946</v>
+        <v>92.482902311963187</v>
       </c>
       <c r="E7">
-        <v>11.65</v>
+        <v>265.10000000000002</v>
       </c>
       <c r="F7">
-        <v>27.55</v>
+        <v>1574.9</v>
       </c>
       <c r="G7">
-        <v>10.85</v>
+        <v>6.75</v>
       </c>
       <c r="H7">
-        <f>AVERAGE(B7,D7,E7,F7,G7)</f>
-        <v>29.83703837119479</v>
+        <f t="shared" si="0"/>
+        <v>324.67363500366054</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B8">
-        <v>4.421215E-3</v>
+        <v>5.7199159999999992E-2</v>
       </c>
       <c r="C8">
-        <v>19.399999999999999</v>
+        <v>80.25</v>
       </c>
       <c r="D8">
-        <v>99.4652416360247</v>
+        <v>95.466460966906681</v>
       </c>
       <c r="E8">
-        <v>12.45</v>
+        <v>235.5</v>
       </c>
       <c r="F8">
-        <v>27.75</v>
+        <v>1610.25</v>
       </c>
       <c r="G8">
-        <v>11.2</v>
+        <v>14.4</v>
       </c>
       <c r="H8">
-        <f>AVERAGE(B8,D8,E8,F8,G8)</f>
-        <v>30.173932570204936</v>
+        <f t="shared" si="0"/>
+        <v>339.32061002115114</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B9">
-        <v>4.4531599999999994E-3</v>
+        <v>9.5076150000000005E-3</v>
       </c>
       <c r="C9">
-        <v>19.399999999999999</v>
+        <v>82.9</v>
       </c>
       <c r="D9">
-        <v>99.4652416360247</v>
+        <v>99.379812332144624</v>
       </c>
       <c r="E9">
-        <v>12.45</v>
+        <v>242.5</v>
       </c>
       <c r="F9">
-        <v>27.75</v>
+        <v>430.7</v>
       </c>
       <c r="G9">
-        <v>11.2</v>
+        <v>13.7</v>
       </c>
       <c r="H9">
-        <f>AVERAGE(B9,D9,E9,F9,G9)</f>
-        <v>30.173938959204939</v>
+        <f t="shared" si="0"/>
+        <v>144.86488665785745</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="B10">
-        <v>5.6002949999999999E-3</v>
+        <v>8.0202699999999995E-3</v>
       </c>
       <c r="C10">
-        <v>9.1999999999999993</v>
+        <v>84.8</v>
       </c>
       <c r="D10">
-        <v>92.764815679459943</v>
+        <v>99.415851301465665</v>
       </c>
       <c r="E10">
-        <v>16.75</v>
+        <v>207.35</v>
       </c>
       <c r="F10">
-        <v>35.049999999999997</v>
+        <v>890.75</v>
       </c>
       <c r="G10">
-        <v>7.2</v>
+        <v>15.95</v>
       </c>
       <c r="H10">
-        <f>AVERAGE(B10,D10,E10,F10,G10)</f>
-        <v>30.354083194891984</v>
+        <f t="shared" si="0"/>
+        <v>216.37897859524426</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B11">
-        <v>5.3238199999999999E-3</v>
+        <v>7.1844350000000003E-3</v>
       </c>
       <c r="C11">
-        <v>11.15</v>
+        <v>9.3000000000000007</v>
       </c>
       <c r="D11">
-        <v>96.401534221050412</v>
+        <v>91.985986402328749</v>
       </c>
       <c r="E11">
-        <v>15.9</v>
+        <v>304.85000000000002</v>
       </c>
       <c r="F11">
-        <v>30.5</v>
+        <v>1118.4000000000001</v>
       </c>
       <c r="G11">
-        <v>9.1</v>
+        <v>7.15</v>
       </c>
       <c r="H11">
-        <f>AVERAGE(B11,D11,E11,F11,G11)</f>
-        <v>30.381371608210081</v>
+        <f t="shared" si="0"/>
+        <v>255.28219513955483</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B12">
-        <v>5.3275099999999997E-3</v>
+        <v>7.1566900000000003E-3</v>
       </c>
       <c r="C12">
-        <v>11.35</v>
+        <v>80.3</v>
       </c>
       <c r="D12">
-        <v>96.811570142749588</v>
+        <v>95.992806563635739</v>
       </c>
       <c r="E12">
-        <v>17.25</v>
+        <v>257.25</v>
       </c>
       <c r="F12">
-        <v>28.95</v>
+        <v>1094.5</v>
       </c>
       <c r="G12">
-        <v>9.3000000000000007</v>
+        <v>12.05</v>
       </c>
       <c r="H12">
-        <f>AVERAGE(B12,D12,E12,F12,G12)</f>
-        <v>30.463379530549918</v>
+        <f t="shared" si="0"/>
+        <v>256.68332720893926</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B13">
-        <v>5.1721400000000004E-3</v>
+        <v>2.8710469999999998E-2</v>
       </c>
       <c r="C13">
-        <v>11.25</v>
+        <v>10.95</v>
       </c>
       <c r="D13">
-        <v>96.40095104720146</v>
+        <v>95.942091919212857</v>
       </c>
       <c r="E13">
-        <v>17.399999999999999</v>
+        <v>228.45</v>
       </c>
       <c r="F13">
-        <v>30.85</v>
+        <v>456.95</v>
       </c>
       <c r="G13">
-        <v>9.15</v>
+        <v>8.8000000000000007</v>
       </c>
       <c r="H13">
-        <f>AVERAGE(B13,D13,E13,F13,G13)</f>
-        <v>30.761224637440289</v>
+        <f t="shared" si="0"/>
+        <v>133.52013373153545</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="B14">
-        <v>6.2039749999999996E-3</v>
+        <v>3.0107795E-2</v>
       </c>
       <c r="C14">
-        <v>10.95</v>
+        <v>88.05</v>
       </c>
       <c r="D14">
-        <v>95.679034212460891</v>
+        <v>102.72798333582161</v>
       </c>
       <c r="E14">
-        <v>17.45</v>
+        <v>229.45</v>
       </c>
       <c r="F14">
-        <v>33.4</v>
+        <v>494</v>
       </c>
       <c r="G14">
-        <v>8.9</v>
+        <v>14.35</v>
       </c>
       <c r="H14">
-        <f>AVERAGE(B14,D14,E14,F14,G14)</f>
-        <v>31.08704763749218</v>
+        <f t="shared" si="0"/>
+        <v>154.76801518847029</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B15">
-        <v>5.5108150000000014E-3</v>
+        <v>3.5589095000000001E-2</v>
       </c>
       <c r="C15">
-        <v>9.75</v>
+        <v>87.2</v>
       </c>
       <c r="D15">
-        <v>99.522392368525942</v>
+        <v>101.5259018078045</v>
       </c>
       <c r="E15">
-        <v>16.95</v>
+        <v>222.45</v>
       </c>
       <c r="F15">
-        <v>32</v>
+        <v>543.5</v>
       </c>
       <c r="G15">
-        <v>7.75</v>
+        <v>14.65</v>
       </c>
       <c r="H15">
-        <f>AVERAGE(B15,D15,E15,F15,G15)</f>
-        <v>31.245580636705188</v>
+        <f t="shared" si="0"/>
+        <v>161.56024848380073</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B16">
-        <v>5.5577200000000004E-3</v>
+        <v>3.9593120000000002E-2</v>
       </c>
       <c r="C16">
-        <v>18.05</v>
+        <v>9.9</v>
       </c>
       <c r="D16">
-        <v>95.466460966906681</v>
+        <v>91.984921200877267</v>
       </c>
       <c r="E16">
-        <v>16.75</v>
+        <v>221.85</v>
       </c>
       <c r="F16">
-        <v>35.049999999999997</v>
+        <v>1060.95</v>
       </c>
       <c r="G16">
-        <v>9.0500000000000007</v>
+        <v>7.9</v>
       </c>
       <c r="H16">
-        <f>AVERAGE(B16,D16,E16,F16,G16)</f>
-        <v>31.264403737381336</v>
+        <f t="shared" si="0"/>
+        <v>232.10408572014623</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B17">
-        <v>5.8817000000000001E-3</v>
+        <v>3.7197380000000002E-2</v>
       </c>
       <c r="C17">
-        <v>11.4</v>
+        <v>81.150000000000006</v>
       </c>
       <c r="D17">
-        <v>99.450828686644769</v>
+        <v>95.993668760770873</v>
       </c>
       <c r="E17">
-        <v>17</v>
+        <v>244.05</v>
       </c>
       <c r="F17">
-        <v>31.1</v>
+        <v>1071</v>
       </c>
       <c r="G17">
-        <v>9.35</v>
+        <v>11.7</v>
       </c>
       <c r="H17">
-        <f>AVERAGE(B17,D17,E17,F17,G17)</f>
-        <v>31.381342077328952</v>
+        <f t="shared" si="0"/>
+        <v>250.65514435679518</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="B18">
-        <v>5.2031300000000003E-3</v>
+        <v>5.3549600000000006E-3</v>
       </c>
       <c r="C18">
-        <v>19.25</v>
+        <v>18.05</v>
       </c>
       <c r="D18">
-        <v>99.623820279787381</v>
+        <v>95.466460966906681</v>
       </c>
       <c r="E18">
-        <v>17.25</v>
+        <v>16.75</v>
       </c>
       <c r="F18">
-        <v>28.95</v>
+        <v>35.049999999999997</v>
       </c>
       <c r="G18">
-        <v>11.6</v>
+        <v>9.0500000000000007</v>
       </c>
       <c r="H18">
-        <f>AVERAGE(B18,D18,E18,F18,G18)</f>
-        <v>31.485804681957472</v>
+        <f t="shared" si="0"/>
+        <v>29.061969321151121</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="B19">
-        <v>5.0595700000000002E-3</v>
+        <v>4.175425E-3</v>
       </c>
       <c r="C19">
-        <v>19.25</v>
+        <v>18.850000000000001</v>
       </c>
       <c r="D19">
-        <v>99.055191129685852</v>
+        <v>99.130927060973946</v>
       </c>
       <c r="E19">
-        <v>17.399999999999999</v>
+        <v>11.65</v>
       </c>
       <c r="F19">
-        <v>30.85</v>
+        <v>27.55</v>
       </c>
       <c r="G19">
-        <v>11.5</v>
+        <v>10.85</v>
       </c>
       <c r="H19">
-        <f>AVERAGE(B19,D19,E19,F19,G19)</f>
-        <v>31.762050139937166</v>
+        <f t="shared" si="0"/>
+        <v>28.005850414328993</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="B20">
-        <v>6.515865E-3</v>
+        <v>6.2702000000000009E-3</v>
       </c>
       <c r="C20">
-        <v>9.9499999999999993</v>
+        <v>17.649999999999999</v>
       </c>
       <c r="D20">
-        <v>94.324349526678361</v>
+        <v>95.905800795126837</v>
       </c>
       <c r="E20">
         <v>15</v>
@@ -1180,686 +1180,686 @@
         <v>41.8</v>
       </c>
       <c r="G20">
-        <v>7.95</v>
+        <v>9.6</v>
       </c>
       <c r="H20">
-        <f>AVERAGE(B20,D20,E20,F20,G20)</f>
-        <v>31.81617307833567</v>
+        <f t="shared" si="0"/>
+        <v>29.993678499187805</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="B21">
-        <v>5.1926000000000003E-3</v>
+        <v>7.9057550000000004E-3</v>
       </c>
       <c r="C21">
-        <v>19.350000000000001</v>
+        <v>9</v>
       </c>
       <c r="D21">
-        <v>102.29869401394031</v>
+        <v>94.129850728560768</v>
       </c>
       <c r="E21">
-        <v>15.9</v>
+        <v>12.25</v>
       </c>
       <c r="F21">
-        <v>30.5</v>
+        <v>46.65</v>
       </c>
       <c r="G21">
-        <v>11.3</v>
+        <v>7</v>
       </c>
       <c r="H21">
-        <f>AVERAGE(B21,D21,E21,F21,G21)</f>
-        <v>32.000777322788068</v>
+        <f t="shared" si="0"/>
+        <v>28.172959413926794</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="B22">
-        <v>8.0527150000000002E-3</v>
+        <v>7.6949650000000007E-3</v>
       </c>
       <c r="C22">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="D22">
-        <v>94.129850728560768</v>
+        <v>96.580674529279761</v>
       </c>
       <c r="E22">
-        <v>12.25</v>
+        <v>12.7</v>
       </c>
       <c r="F22">
-        <v>46.65</v>
+        <v>46</v>
       </c>
       <c r="G22">
-        <v>7</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="H22">
-        <f>AVERAGE(B22,D22,E22,F22,G22)</f>
-        <v>32.007580688712153</v>
+        <f t="shared" si="0"/>
+        <v>30.414728249046629</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B23">
-        <v>6.6467650000000007E-3</v>
+        <v>5.7396324999999991E-2</v>
       </c>
       <c r="C23">
-        <v>10.5</v>
+        <v>8.8000000000000007</v>
       </c>
       <c r="D23">
-        <v>95.302702649425811</v>
+        <v>92.33396854170924</v>
       </c>
       <c r="E23">
-        <v>14.75</v>
+        <v>235.5</v>
       </c>
       <c r="F23">
-        <v>42.05</v>
+        <v>1610.25</v>
       </c>
       <c r="G23">
-        <v>8.5</v>
+        <v>6.75</v>
       </c>
       <c r="H23">
-        <f>AVERAGE(B23,D23,E23,F23,G23)</f>
-        <v>32.121869882885164</v>
+        <f t="shared" si="0"/>
+        <v>325.61522747778486</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="B24">
-        <v>7.8713350000000001E-3</v>
+        <v>9.8343599999999986E-3</v>
       </c>
       <c r="C24">
-        <v>9.6999999999999993</v>
+        <v>10.7</v>
       </c>
       <c r="D24">
-        <v>95.244064290933849</v>
+        <v>95.051447410283174</v>
       </c>
       <c r="E24">
-        <v>12.7</v>
+        <v>242.5</v>
       </c>
       <c r="F24">
-        <v>46</v>
+        <v>430.7</v>
       </c>
       <c r="G24">
-        <v>7.7</v>
+        <v>8.5500000000000007</v>
       </c>
       <c r="H24">
-        <f>AVERAGE(B24,D24,E24,F24,G24)</f>
-        <v>32.330387125186768</v>
+        <f t="shared" si="0"/>
+        <v>131.25188029504719</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B25">
-        <v>6.0305100000000002E-3</v>
+        <v>1.011546E-2</v>
       </c>
       <c r="C25">
-        <v>19.399999999999999</v>
+        <v>83.9</v>
       </c>
       <c r="D25">
-        <v>100.0149891043306</v>
+        <v>100.3383909759073</v>
       </c>
       <c r="E25">
-        <v>17.45</v>
+        <v>231.4</v>
       </c>
       <c r="F25">
-        <v>33.4</v>
+        <v>471.3</v>
       </c>
       <c r="G25">
-        <v>10.9</v>
+        <v>13.4</v>
       </c>
       <c r="H25">
-        <f>AVERAGE(B25,D25,E25,F25,G25)</f>
-        <v>32.35420392286612</v>
+        <f t="shared" si="0"/>
+        <v>150.05808440598454</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B26">
-        <v>6.3632899999999989E-3</v>
+        <v>1.482062E-2</v>
       </c>
       <c r="C26">
-        <v>9.8000000000000007</v>
+        <v>86.2</v>
       </c>
       <c r="D26">
-        <v>98.600668691583124</v>
+        <v>100.5259018078045</v>
       </c>
       <c r="E26">
-        <v>17.850000000000001</v>
+        <v>217.9</v>
       </c>
       <c r="F26">
-        <v>37.700000000000003</v>
+        <v>528.20000000000005</v>
       </c>
       <c r="G26">
-        <v>7.8</v>
+        <v>14.4</v>
       </c>
       <c r="H26">
-        <f>AVERAGE(B26,D26,E26,F26,G26)</f>
-        <v>32.391406396316633</v>
+        <f t="shared" si="0"/>
+        <v>157.87345373796742</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B27">
-        <v>6.3895249999999983E-3</v>
+        <v>8.3724000000000003E-3</v>
       </c>
       <c r="C27">
-        <v>17.649999999999999</v>
+        <v>11.65</v>
       </c>
       <c r="D27">
-        <v>95.905800795126837</v>
+        <v>94.96604375813385</v>
       </c>
       <c r="E27">
-        <v>15</v>
+        <v>207.35</v>
       </c>
       <c r="F27">
-        <v>41.8</v>
+        <v>890.75</v>
       </c>
       <c r="G27">
-        <v>9.6</v>
+        <v>9.3000000000000007</v>
       </c>
       <c r="H27">
-        <f>AVERAGE(B27,D27,E27,F27,G27)</f>
-        <v>32.462438064025363</v>
+        <f t="shared" si="0"/>
+        <v>202.33740269302231</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="B28">
-        <v>5.4206050000000002E-3</v>
+        <v>8.2059100000000003E-3</v>
       </c>
       <c r="C28">
-        <v>18.7</v>
+        <v>84.85</v>
       </c>
       <c r="D28">
-        <v>103.8058007951268</v>
+        <v>99.652247404533583</v>
       </c>
       <c r="E28">
-        <v>16.95</v>
+        <v>214.7</v>
       </c>
       <c r="F28">
-        <v>32</v>
+        <v>903.35</v>
       </c>
       <c r="G28">
-        <v>9.65</v>
+        <v>16</v>
       </c>
       <c r="H28">
-        <f>AVERAGE(B28,D28,E28,F28,G28)</f>
-        <v>32.482244280025363</v>
+        <f t="shared" si="0"/>
+        <v>219.76007555242225</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="B29">
-        <v>5.7433099999999997E-3</v>
+        <v>7.5084250000000009E-3</v>
       </c>
       <c r="C29">
-        <v>19.25</v>
+        <v>9.0500000000000007</v>
       </c>
       <c r="D29">
-        <v>103.10960671741429</v>
+        <v>92.206496440983841</v>
       </c>
       <c r="E29">
-        <v>17</v>
+        <v>257.25</v>
       </c>
       <c r="F29">
-        <v>31.1</v>
+        <v>1094.5</v>
       </c>
       <c r="G29">
-        <v>11.65</v>
+        <v>7</v>
       </c>
       <c r="H29">
-        <f>AVERAGE(B29,D29,E29,F29,G29)</f>
-        <v>32.573070005482862</v>
+        <f t="shared" si="0"/>
+        <v>243.33566747766397</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B30">
-        <v>7.9309800000000007E-3</v>
+        <v>3.043096E-2</v>
       </c>
       <c r="C30">
-        <v>17.149999999999999</v>
+        <v>10.7</v>
       </c>
       <c r="D30">
-        <v>95.466460966906681</v>
+        <v>97.115190628049064</v>
       </c>
       <c r="E30">
-        <v>12.25</v>
+        <v>229.45</v>
       </c>
       <c r="F30">
-        <v>46.65</v>
+        <v>494</v>
       </c>
       <c r="G30">
-        <v>8.5</v>
+        <v>8.6</v>
       </c>
       <c r="H30">
-        <f>AVERAGE(B30,D30,E30,F30,G30)</f>
-        <v>32.57487838938134</v>
+        <f t="shared" si="0"/>
+        <v>139.98260359800818</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B31">
-        <v>6.5722000000000003E-3</v>
+        <v>3.5856364999999987E-2</v>
       </c>
       <c r="C31">
-        <v>18.649999999999999</v>
+        <v>11.35</v>
       </c>
       <c r="D31">
-        <v>97.195750288788005</v>
+        <v>96.470693022813506</v>
       </c>
       <c r="E31">
-        <v>14.75</v>
+        <v>222.45</v>
       </c>
       <c r="F31">
-        <v>42.05</v>
+        <v>543.5</v>
       </c>
       <c r="G31">
-        <v>10.25</v>
+        <v>9.35</v>
       </c>
       <c r="H31">
-        <f>AVERAGE(B31,D31,E31,F31,G31)</f>
-        <v>32.850464497757599</v>
+        <f t="shared" si="0"/>
+        <v>147.19275823130224</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B32">
-        <v>7.8366550000000014E-3</v>
+        <v>3.433538500000001E-2</v>
       </c>
       <c r="C32">
-        <v>18</v>
+        <v>86.65</v>
       </c>
       <c r="D32">
-        <v>96.580674529279761</v>
+        <v>100.706662992262</v>
       </c>
       <c r="E32">
-        <v>12.7</v>
+        <v>223.4</v>
       </c>
       <c r="F32">
-        <v>46</v>
+        <v>536.6</v>
       </c>
       <c r="G32">
-        <v>9.1999999999999993</v>
+        <v>13.9</v>
       </c>
       <c r="H32">
-        <f>AVERAGE(B32,D32,E32,F32,G32)</f>
-        <v>32.897702236855949</v>
+        <f t="shared" si="0"/>
+        <v>160.21516639621032</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="B33">
-        <v>6.2852400000000001E-3</v>
+        <v>3.7452159999999998E-2</v>
       </c>
       <c r="C33">
-        <v>18.649999999999999</v>
+        <v>9.9</v>
       </c>
       <c r="D33">
-        <v>101.706662992262</v>
+        <v>92.095917778269126</v>
       </c>
       <c r="E33">
-        <v>17.850000000000001</v>
+        <v>244.05</v>
       </c>
       <c r="F33">
-        <v>37.700000000000003</v>
+        <v>1071</v>
       </c>
       <c r="G33">
-        <v>9.6</v>
+        <v>7.85</v>
       </c>
       <c r="H33">
-        <f>AVERAGE(B33,D33,E33,F33,G33)</f>
-        <v>33.372589646452397</v>
+        <f t="shared" si="0"/>
+        <v>237.48889498971153</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="B34">
-        <v>1.0104284999999999E-2</v>
+        <v>5.0496500000000001E-3</v>
       </c>
       <c r="C34">
-        <v>10.7</v>
+        <v>19.350000000000001</v>
       </c>
       <c r="D34">
-        <v>95.051447410283174</v>
+        <v>102.29869401394031</v>
       </c>
       <c r="E34">
-        <v>242.5</v>
+        <v>15.9</v>
       </c>
       <c r="F34">
-        <v>430.7</v>
+        <v>30.5</v>
       </c>
       <c r="G34">
-        <v>8.5500000000000007</v>
+        <v>11.3</v>
       </c>
       <c r="H34">
-        <f>AVERAGE(B34,D34,E34,F34,G34)</f>
-        <v>155.36231033905662</v>
+        <f t="shared" si="0"/>
+        <v>29.892290610656719</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="B35">
-        <v>9.6960650000000002E-3</v>
+        <v>4.9714599999999996E-3</v>
       </c>
       <c r="C35">
-        <v>82.9</v>
+        <v>19.25</v>
       </c>
       <c r="D35">
-        <v>99.379812332144624</v>
+        <v>99.055191129685852</v>
       </c>
       <c r="E35">
-        <v>242.5</v>
+        <v>17.399999999999999</v>
       </c>
       <c r="F35">
-        <v>430.7</v>
+        <v>30.85</v>
       </c>
       <c r="G35">
-        <v>13.7</v>
+        <v>11.5</v>
       </c>
       <c r="H35">
-        <f>AVERAGE(B35,D35,E35,F35,G35)</f>
-        <v>157.25790167942893</v>
+        <f t="shared" si="0"/>
+        <v>29.676693764947643</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>56</v>
+        <v>41</v>
       </c>
       <c r="B36">
-        <v>2.9022179999999991E-2</v>
+        <v>5.4570399999999989E-3</v>
       </c>
       <c r="C36">
-        <v>10.95</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="D36">
-        <v>95.942091919212857</v>
+        <v>92.764815679459943</v>
       </c>
       <c r="E36">
-        <v>228.45</v>
+        <v>16.75</v>
       </c>
       <c r="F36">
-        <v>456.95</v>
+        <v>35.049999999999997</v>
       </c>
       <c r="G36">
-        <v>8.8000000000000007</v>
+        <v>7.2</v>
       </c>
       <c r="H36">
-        <f>AVERAGE(B36,D36,E36,F36,G36)</f>
-        <v>158.03422281984257</v>
+        <f t="shared" si="0"/>
+        <v>26.828378786576653</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="B37">
-        <v>2.8768245000000001E-2</v>
+        <v>6.1662299999999991E-3</v>
       </c>
       <c r="C37">
-        <v>86.95</v>
+        <v>18.649999999999999</v>
       </c>
       <c r="D37">
-        <v>101.545140623347</v>
+        <v>101.706662992262</v>
       </c>
       <c r="E37">
-        <v>228.45</v>
+        <v>17.850000000000001</v>
       </c>
       <c r="F37">
-        <v>456.95</v>
+        <v>37.700000000000003</v>
       </c>
       <c r="G37">
-        <v>16.7</v>
+        <v>9.6</v>
       </c>
       <c r="H37">
-        <f>AVERAGE(B37,D37,E37,F37,G37)</f>
-        <v>160.73478177366943</v>
+        <f t="shared" si="0"/>
+        <v>30.918804870377002</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="B38">
-        <v>1.066193E-2</v>
+        <v>4.2538850000000007E-3</v>
       </c>
       <c r="C38">
-        <v>10.6</v>
+        <v>11</v>
       </c>
       <c r="D38">
-        <v>96.262525712883303</v>
+        <v>97.253304076183326</v>
       </c>
       <c r="E38">
-        <v>231.4</v>
+        <v>11.65</v>
       </c>
       <c r="F38">
-        <v>471.3</v>
+        <v>27.55</v>
       </c>
       <c r="G38">
-        <v>8.4</v>
+        <v>9</v>
       </c>
       <c r="H38">
-        <f>AVERAGE(B38,D38,E38,F38,G38)</f>
-        <v>161.47463752857666</v>
+        <f t="shared" si="0"/>
+        <v>26.076259660197223</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B39">
-        <v>1.0365640000000001E-2</v>
+        <v>4.0263149999999999E-3</v>
       </c>
       <c r="C39">
-        <v>83.9</v>
+        <v>18.850000000000001</v>
       </c>
       <c r="D39">
-        <v>100.3383909759073</v>
+        <v>99.130927060973946</v>
       </c>
       <c r="E39">
-        <v>231.4</v>
+        <v>11.75</v>
       </c>
       <c r="F39">
-        <v>471.3</v>
+        <v>26.95</v>
       </c>
       <c r="G39">
-        <v>13.4</v>
+        <v>10.85</v>
       </c>
       <c r="H39">
-        <f>AVERAGE(B39,D39,E39,F39,G39)</f>
-        <v>163.28975132318146</v>
+        <f t="shared" si="0"/>
+        <v>27.922492229328984</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="B40">
-        <v>3.0900194999999998E-2</v>
+        <v>4.3084050000000004E-3</v>
       </c>
       <c r="C40">
-        <v>10.7</v>
+        <v>19.399999999999999</v>
       </c>
       <c r="D40">
-        <v>97.115190628049064</v>
+        <v>99.4652416360247</v>
       </c>
       <c r="E40">
-        <v>229.45</v>
+        <v>12.45</v>
       </c>
       <c r="F40">
-        <v>494</v>
+        <v>27.75</v>
       </c>
       <c r="G40">
-        <v>8.6</v>
+        <v>11.2</v>
       </c>
       <c r="H40">
-        <f>AVERAGE(B40,D40,E40,F40,G40)</f>
-        <v>165.8392181646098</v>
+        <f t="shared" si="0"/>
+        <v>28.378258340170778</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="B41">
-        <v>3.043255499999999E-2</v>
+        <v>6.3522550000000011E-3</v>
       </c>
       <c r="C41">
-        <v>88.05</v>
+        <v>9.9499999999999993</v>
       </c>
       <c r="D41">
-        <v>102.72798333582161</v>
+        <v>94.324349526678361</v>
       </c>
       <c r="E41">
-        <v>229.45</v>
+        <v>15</v>
       </c>
       <c r="F41">
-        <v>494</v>
+        <v>41.8</v>
       </c>
       <c r="G41">
-        <v>14.35</v>
+        <v>7.95</v>
       </c>
       <c r="H41">
-        <f>AVERAGE(B41,D41,E41,F41,G41)</f>
-        <v>168.11168317816433</v>
+        <f t="shared" si="0"/>
+        <v>28.171783630279723</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="B42">
-        <v>1.5421974999999999E-2</v>
+        <v>6.4687750000000004E-3</v>
       </c>
       <c r="C42">
-        <v>11.2</v>
+        <v>18.649999999999999</v>
       </c>
       <c r="D42">
-        <v>96.304366757830977</v>
+        <v>97.195750288788005</v>
       </c>
       <c r="E42">
-        <v>217.9</v>
+        <v>14.75</v>
       </c>
       <c r="F42">
-        <v>528.20000000000005</v>
+        <v>42.05</v>
       </c>
       <c r="G42">
-        <v>9.15</v>
+        <v>10.25</v>
       </c>
       <c r="H42">
-        <f>AVERAGE(B42,D42,E42,F42,G42)</f>
-        <v>170.31395774656619</v>
+        <f t="shared" si="0"/>
+        <v>30.483703177297997</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B43">
-        <v>1.4684525E-2</v>
+        <v>7.7220349999999986E-3</v>
       </c>
       <c r="C43">
-        <v>11.2</v>
+        <v>9.6999999999999993</v>
       </c>
       <c r="D43">
-        <v>96.11554805056582</v>
+        <v>95.244064290933849</v>
       </c>
       <c r="E43">
-        <v>232.5</v>
+        <v>12.7</v>
       </c>
       <c r="F43">
-        <v>522.54999999999995</v>
+        <v>46</v>
       </c>
       <c r="G43">
-        <v>9.1</v>
+        <v>7.7</v>
       </c>
       <c r="H43">
-        <f>AVERAGE(B43,D43,E43,F43,G43)</f>
-        <v>172.05604651511317</v>
+        <f t="shared" si="0"/>
+        <v>28.558631054322309</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B44">
-        <v>1.5087895E-2</v>
+        <v>1.0459725E-2</v>
       </c>
       <c r="C44">
-        <v>86.2</v>
+        <v>10.6</v>
       </c>
       <c r="D44">
-        <v>100.5259018078045</v>
+        <v>96.262525712883303</v>
       </c>
       <c r="E44">
-        <v>217.9</v>
+        <v>231.4</v>
       </c>
       <c r="F44">
-        <v>528.20000000000005</v>
+        <v>471.3</v>
       </c>
       <c r="G44">
-        <v>14.4</v>
+        <v>8.4</v>
       </c>
       <c r="H44">
-        <f>AVERAGE(B44,D44,E44,F44,G44)</f>
-        <v>172.20819794056089</v>
+        <f t="shared" si="0"/>
+        <v>136.32883090631387</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="B45">
-        <v>3.5119934999999998E-2</v>
+        <v>1.5185805E-2</v>
       </c>
       <c r="C45">
-        <v>11.15</v>
+        <v>11.2</v>
       </c>
       <c r="D45">
-        <v>96.343053687454997</v>
+        <v>96.304366757830977</v>
       </c>
       <c r="E45">
-        <v>223.4</v>
+        <v>217.9</v>
       </c>
       <c r="F45">
-        <v>536.6</v>
+        <v>528.20000000000005</v>
       </c>
       <c r="G45">
-        <v>9.1</v>
+        <v>9.15</v>
       </c>
       <c r="H45">
-        <f>AVERAGE(B45,D45,E45,F45,G45)</f>
-        <v>173.09563472449102</v>
+        <f t="shared" si="0"/>
+        <v>143.79492542713851</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.3">
@@ -1867,7 +1867,7 @@
         <v>51</v>
       </c>
       <c r="B46">
-        <v>1.428571E-2</v>
+        <v>1.402522E-2</v>
       </c>
       <c r="C46">
         <v>85.45</v>
@@ -1885,49 +1885,49 @@
         <v>13.95</v>
       </c>
       <c r="H46">
-        <f>AVERAGE(B46,D46,E46,F46,G46)</f>
-        <v>173.82016953791685</v>
+        <f t="shared" si="0"/>
+        <v>159.09176453326404</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="B47">
-        <v>3.6348114999999993E-2</v>
+        <v>8.5663300000000005E-3</v>
       </c>
       <c r="C47">
-        <v>11.35</v>
+        <v>11.55</v>
       </c>
       <c r="D47">
-        <v>96.470693022813506</v>
+        <v>94.983149630726132</v>
       </c>
       <c r="E47">
-        <v>222.45</v>
+        <v>214.7</v>
       </c>
       <c r="F47">
-        <v>543.5</v>
+        <v>903.35</v>
       </c>
       <c r="G47">
-        <v>9.35</v>
+        <v>9.25</v>
       </c>
       <c r="H47">
-        <f>AVERAGE(B47,D47,E47,F47,G47)</f>
-        <v>174.36140822756269</v>
+        <f t="shared" si="0"/>
+        <v>205.64028599345434</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="B48">
-        <v>3.4740115000000002E-2</v>
+        <v>3.4688625000000001E-2</v>
       </c>
       <c r="C48">
-        <v>86.65</v>
+        <v>11.15</v>
       </c>
       <c r="D48">
-        <v>100.706662992262</v>
+        <v>96.343053687454997</v>
       </c>
       <c r="E48">
         <v>223.4</v>
@@ -1936,389 +1936,389 @@
         <v>536.6</v>
       </c>
       <c r="G48">
-        <v>13.9</v>
+        <v>9.1</v>
       </c>
       <c r="H48">
-        <f>AVERAGE(B48,D48,E48,F48,G48)</f>
-        <v>174.92828062145242</v>
+        <f t="shared" si="0"/>
+        <v>146.10462371874252</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="B49">
-        <v>3.6140159999999998E-2</v>
+        <v>5.1678550000000007E-3</v>
       </c>
       <c r="C49">
-        <v>87.2</v>
+        <v>11.15</v>
       </c>
       <c r="D49">
-        <v>101.5259018078045</v>
+        <v>96.401534221050412</v>
       </c>
       <c r="E49">
-        <v>222.45</v>
+        <v>15.9</v>
       </c>
       <c r="F49">
-        <v>543.5</v>
+        <v>30.5</v>
       </c>
       <c r="G49">
-        <v>14.65</v>
+        <v>9.1</v>
       </c>
       <c r="H49">
-        <f>AVERAGE(B49,D49,E49,F49,G49)</f>
-        <v>176.43240839356091</v>
+        <f t="shared" si="0"/>
+        <v>27.176117012675068</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="B50">
-        <v>8.5732799999999991E-3</v>
+        <v>5.3185200000000002E-3</v>
       </c>
       <c r="C50">
-        <v>11.65</v>
+        <v>18.7</v>
       </c>
       <c r="D50">
-        <v>94.96604375813385</v>
+        <v>103.8058007951268</v>
       </c>
       <c r="E50">
-        <v>207.35</v>
+        <v>16.95</v>
       </c>
       <c r="F50">
-        <v>890.75</v>
+        <v>32</v>
       </c>
       <c r="G50">
-        <v>9.3000000000000007</v>
+        <v>9.65</v>
       </c>
       <c r="H50">
-        <f>AVERAGE(B50,D50,E50,F50,G50)</f>
-        <v>240.47492340762679</v>
+        <f t="shared" si="0"/>
+        <v>30.185186552521131</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="B51">
-        <v>8.1824249999999984E-3</v>
+        <v>5.0783499999999997E-3</v>
       </c>
       <c r="C51">
-        <v>84.8</v>
+        <v>19.25</v>
       </c>
       <c r="D51">
-        <v>99.415851301465665</v>
+        <v>99.623820279787381</v>
       </c>
       <c r="E51">
-        <v>207.35</v>
+        <v>17.25</v>
       </c>
       <c r="F51">
-        <v>890.75</v>
+        <v>28.95</v>
       </c>
       <c r="G51">
-        <v>15.95</v>
+        <v>11.6</v>
       </c>
       <c r="H51">
-        <f>AVERAGE(B51,D51,E51,F51,G51)</f>
-        <v>242.69480674529314</v>
+        <f t="shared" si="0"/>
+        <v>29.44648310496456</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="B52">
-        <v>8.7415349999999999E-3</v>
+        <v>5.0669699999999996E-3</v>
       </c>
       <c r="C52">
-        <v>11.55</v>
+        <v>11.25</v>
       </c>
       <c r="D52">
-        <v>94.983149630726132</v>
+        <v>96.40095104720146</v>
       </c>
       <c r="E52">
-        <v>214.7</v>
+        <v>17.399999999999999</v>
       </c>
       <c r="F52">
-        <v>903.35</v>
+        <v>30.85</v>
       </c>
       <c r="G52">
-        <v>9.25</v>
+        <v>9.15</v>
       </c>
       <c r="H52">
-        <f>AVERAGE(B52,D52,E52,F52,G52)</f>
-        <v>244.45837823314523</v>
+        <f t="shared" si="0"/>
+        <v>27.509336336200246</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>44</v>
+        <v>58</v>
       </c>
       <c r="B53">
-        <v>8.4723699999999999E-3</v>
+        <v>5.917630000000001E-3</v>
       </c>
       <c r="C53">
-        <v>84.85</v>
+        <v>19.399999999999999</v>
       </c>
       <c r="D53">
-        <v>99.652247404533583</v>
+        <v>100.0149891043306</v>
       </c>
       <c r="E53">
-        <v>214.7</v>
+        <v>17.45</v>
       </c>
       <c r="F53">
-        <v>903.35</v>
+        <v>33.4</v>
       </c>
       <c r="G53">
-        <v>16</v>
+        <v>10.9</v>
       </c>
       <c r="H53">
-        <f>AVERAGE(B53,D53,E53,F53,G53)</f>
-        <v>246.74214395490671</v>
+        <f t="shared" si="0"/>
+        <v>30.195151122388435</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="B54">
-        <v>4.0010909999999997E-2</v>
+        <v>6.2643300000000002E-3</v>
       </c>
       <c r="C54">
-        <v>9.9</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="D54">
-        <v>91.984921200877267</v>
+        <v>98.600668691583124</v>
       </c>
       <c r="E54">
-        <v>221.85</v>
+        <v>17.850000000000001</v>
       </c>
       <c r="F54">
-        <v>1060.95</v>
+        <v>37.700000000000003</v>
       </c>
       <c r="G54">
-        <v>7.9</v>
+        <v>7.8</v>
       </c>
       <c r="H54">
-        <f>AVERAGE(B54,D54,E54,F54,G54)</f>
-        <v>276.5449864221755</v>
+        <f t="shared" si="0"/>
+        <v>28.626155503597193</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="B55">
-        <v>3.9660354999999987E-2</v>
+        <v>4.1219049999999986E-3</v>
       </c>
       <c r="C55">
-        <v>80.95</v>
+        <v>11</v>
       </c>
       <c r="D55">
-        <v>95.8765114732455</v>
+        <v>97.253304076183326</v>
       </c>
       <c r="E55">
-        <v>221.85</v>
+        <v>11.75</v>
       </c>
       <c r="F55">
-        <v>1060.95</v>
+        <v>26.95</v>
       </c>
       <c r="G55">
-        <v>11.7</v>
+        <v>9</v>
       </c>
       <c r="H55">
-        <f>AVERAGE(B55,D55,E55,F55,G55)</f>
-        <v>278.0832343656491</v>
+        <f t="shared" si="0"/>
+        <v>25.99290433019722</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B56">
-        <v>3.7843990000000008E-2</v>
+        <v>4.4020500000000002E-3</v>
       </c>
       <c r="C56">
-        <v>9.9</v>
+        <v>11.4</v>
       </c>
       <c r="D56">
-        <v>92.095917778269126</v>
+        <v>97.581102103629476</v>
       </c>
       <c r="E56">
-        <v>244.05</v>
+        <v>12.45</v>
       </c>
       <c r="F56">
-        <v>1071</v>
+        <v>27.75</v>
       </c>
       <c r="G56">
-        <v>7.85</v>
+        <v>9.4</v>
       </c>
       <c r="H56">
-        <f>AVERAGE(B56,D56,E56,F56,G56)</f>
-        <v>283.00675235365378</v>
+        <f t="shared" si="0"/>
+        <v>26.430917358938249</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B57">
-        <v>3.7584480000000003E-2</v>
+        <v>4.3338500000000002E-3</v>
       </c>
       <c r="C57">
-        <v>81.150000000000006</v>
+        <v>19.399999999999999</v>
       </c>
       <c r="D57">
-        <v>95.993668760770873</v>
+        <v>99.4652416360247</v>
       </c>
       <c r="E57">
-        <v>244.05</v>
+        <v>12.45</v>
       </c>
       <c r="F57">
-        <v>1071</v>
+        <v>27.75</v>
       </c>
       <c r="G57">
-        <v>11.7</v>
+        <v>11.2</v>
       </c>
       <c r="H57">
-        <f>AVERAGE(B57,D57,E57,F57,G57)</f>
-        <v>284.55625064815416</v>
+        <f t="shared" si="0"/>
+        <v>28.378262581004112</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>38</v>
+        <v>63</v>
       </c>
       <c r="B58">
-        <v>7.6447499999999988E-3</v>
+        <v>6.5454250000000014E-3</v>
       </c>
       <c r="C58">
-        <v>9.0500000000000007</v>
+        <v>10.5</v>
       </c>
       <c r="D58">
-        <v>92.206496440983841</v>
+        <v>95.302702649425811</v>
       </c>
       <c r="E58">
-        <v>257.25</v>
+        <v>14.75</v>
       </c>
       <c r="F58">
-        <v>1094.5</v>
+        <v>42.05</v>
       </c>
       <c r="G58">
-        <v>7</v>
+        <v>8.5</v>
       </c>
       <c r="H58">
-        <f>AVERAGE(B58,D58,E58,F58,G58)</f>
-        <v>290.19282823819674</v>
+        <f t="shared" si="0"/>
+        <v>28.518208012404301</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>37</v>
+        <v>64</v>
       </c>
       <c r="B59">
-        <v>7.4067350000000002E-3</v>
+        <v>1.439782E-2</v>
       </c>
       <c r="C59">
-        <v>80.3</v>
+        <v>11.2</v>
       </c>
       <c r="D59">
-        <v>95.992806563635739</v>
+        <v>96.11554805056582</v>
       </c>
       <c r="E59">
-        <v>257.25</v>
+        <v>232.5</v>
       </c>
       <c r="F59">
-        <v>1094.5</v>
+        <v>522.54999999999995</v>
       </c>
       <c r="G59">
-        <v>12.05</v>
+        <v>9.1</v>
       </c>
       <c r="H59">
-        <f>AVERAGE(B59,D59,E59,F59,G59)</f>
-        <v>291.96004265972715</v>
+        <f t="shared" si="0"/>
+        <v>145.2466576450943</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>36</v>
+        <v>65</v>
       </c>
       <c r="B60">
-        <v>7.3918600000000001E-3</v>
+        <v>5.3969999999999999E-3</v>
       </c>
       <c r="C60">
-        <v>9.3000000000000007</v>
+        <v>9.75</v>
       </c>
       <c r="D60">
-        <v>91.985986402328749</v>
+        <v>99.522392368525942</v>
       </c>
       <c r="E60">
-        <v>304.85000000000002</v>
+        <v>16.95</v>
       </c>
       <c r="F60">
-        <v>1118.4000000000001</v>
+        <v>32</v>
       </c>
       <c r="G60">
-        <v>7.15</v>
+        <v>7.75</v>
       </c>
       <c r="H60">
-        <f>AVERAGE(B60,D60,E60,F60,G60)</f>
-        <v>304.47867565246577</v>
+        <f t="shared" si="0"/>
+        <v>27.662964894754325</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>35</v>
+        <v>66</v>
       </c>
       <c r="B61">
-        <v>6.95402E-3</v>
+        <v>5.1823800000000003E-3</v>
       </c>
       <c r="C61">
-        <v>80.25</v>
+        <v>11.35</v>
       </c>
       <c r="D61">
-        <v>96.046359954229004</v>
+        <v>96.811570142749588</v>
       </c>
       <c r="E61">
-        <v>304.85000000000002</v>
+        <v>17.25</v>
       </c>
       <c r="F61">
-        <v>1118.4000000000001</v>
+        <v>28.95</v>
       </c>
       <c r="G61">
-        <v>12.6</v>
+        <v>9.3000000000000007</v>
       </c>
       <c r="H61">
-        <f>AVERAGE(B61,D61,E61,F61,G61)</f>
-        <v>306.38066279484582</v>
+        <f t="shared" si="0"/>
+        <v>27.277792087124933</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B62">
-        <v>5.9110425000000001E-2</v>
+        <v>5.6154550000000001E-3</v>
       </c>
       <c r="C62">
-        <v>8.75</v>
+        <v>19.25</v>
       </c>
       <c r="D62">
-        <v>92.482902311963187</v>
+        <v>103.10960671741429</v>
       </c>
       <c r="E62">
-        <v>265.10000000000002</v>
+        <v>17</v>
       </c>
       <c r="F62">
-        <v>1574.9</v>
+        <v>31.1</v>
       </c>
       <c r="G62">
-        <v>6.75</v>
+        <v>11.65</v>
       </c>
       <c r="H62">
-        <f>AVERAGE(B62,D62,E62,F62,G62)</f>
-        <v>387.8584025473927</v>
+        <f t="shared" si="0"/>
+        <v>30.352537028735714</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.3">
@@ -2326,26 +2326,26 @@
         <v>68</v>
       </c>
       <c r="B63">
-        <v>5.7648585000000002E-2</v>
+        <v>6.0128149999999986E-3</v>
       </c>
       <c r="C63">
-        <v>8.8000000000000007</v>
+        <v>10.95</v>
       </c>
       <c r="D63">
-        <v>92.33396854170924</v>
+        <v>95.679034212460891</v>
       </c>
       <c r="E63">
-        <v>235.5</v>
+        <v>17.45</v>
       </c>
       <c r="F63">
-        <v>1610.25</v>
+        <v>33.4</v>
       </c>
       <c r="G63">
-        <v>6.75</v>
+        <v>8.9</v>
       </c>
       <c r="H63">
-        <f>AVERAGE(B63,D63,E63,F63,G63)</f>
-        <v>388.97832342534184</v>
+        <f t="shared" si="0"/>
+        <v>27.730841171243483</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.3">
@@ -2353,61 +2353,57 @@
         <v>69</v>
       </c>
       <c r="B64">
-        <v>5.8849354999999992E-2</v>
+        <v>4.4211700000000003E-3</v>
       </c>
       <c r="C64">
-        <v>80.25</v>
+        <v>11.4</v>
       </c>
       <c r="D64">
-        <v>95.466460966906681</v>
+        <v>97.581102103629476</v>
       </c>
       <c r="E64">
-        <v>265.10000000000002</v>
+        <v>12.45</v>
       </c>
       <c r="F64">
-        <v>1574.9</v>
+        <v>27.75</v>
       </c>
       <c r="G64">
-        <v>19.8</v>
+        <v>9.4</v>
       </c>
       <c r="H64">
-        <f>AVERAGE(B64,D64,E64,F64,G64)</f>
-        <v>391.06506206438132</v>
+        <f t="shared" si="0"/>
+        <v>26.430920545604916</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="B65">
-        <v>5.7384484999999999E-2</v>
+        <v>5.7693950000000009E-3</v>
       </c>
       <c r="C65">
-        <v>80.25</v>
+        <v>11.4</v>
       </c>
       <c r="D65">
-        <v>95.466460966906681</v>
+        <v>99.450828686644769</v>
       </c>
       <c r="E65">
-        <v>235.5</v>
+        <v>17</v>
       </c>
       <c r="F65">
-        <v>1610.25</v>
+        <v>31.1</v>
       </c>
       <c r="G65">
-        <v>14.4</v>
+        <v>9.35</v>
       </c>
       <c r="H65">
-        <f>AVERAGE(B65,D65,E65,F65,G65)</f>
-        <v>391.13476909038138</v>
+        <f t="shared" si="0"/>
+        <v>28.051099680274124</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H65" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H65">
-      <sortCondition ref="H1:H65"/>
-    </sortState>
-  </autoFilter>
+  <autoFilter ref="A1:H65" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>